<commit_message>
rajout de navbar. rajout de subscriptions (view, form, templates) pour la gestion des abonnements de l'utilisateur
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LITReviewWebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EE5B99-EC4B-4B75-9259-A0CFAA6C6591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5729A668-12C7-4C96-A1B3-26670EE161FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>admin</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>toto123456</t>
+  </si>
+  <si>
+    <t>foo123</t>
+  </si>
+  <si>
+    <t>foo123456</t>
+  </si>
+  <si>
+    <t>boo123</t>
+  </si>
+  <si>
+    <t>boo123456</t>
   </si>
 </sst>
 </file>
@@ -375,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,6 +434,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mise a jour navbar avec des liens vers la page d'abonnements, mise a jour de views, forms pour la création d'abonnements
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LITReviewWebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5729A668-12C7-4C96-A1B3-26670EE161FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB0DDA5-6861-4395-B81B-A93358DD2ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>admin</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>boo123456</t>
+  </si>
+  <si>
+    <t>zou123</t>
+  </si>
+  <si>
+    <t>zou123456</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,6 +456,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rajout des fonctionnalité de création, suppression, et mise à jour de ticket et review
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LITReviewWebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB0DDA5-6861-4395-B81B-A93358DD2ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490F50B9-61C7-43D5-910B-E6A43F9D35AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
tests, adding posts, tickets
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LITReviewWebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490F50B9-61C7-43D5-910B-E6A43F9D35AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4B6AFE-861F-4CEC-BB2A-29F48D7C059F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>admin</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>zou123456</t>
+  </si>
+  <si>
+    <t>Remarque</t>
   </si>
 </sst>
 </file>
@@ -393,18 +396,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="21.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -417,8 +421,11 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +438,11 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -440,7 +450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -448,7 +458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -456,7 +466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>